<commit_message>
Settings Add departments screen script started and completed the add departments script
</commit_message>
<xml_diff>
--- a/com.SmartGatePuls.SDET/src/Automation.xlsx
+++ b/com.SmartGatePuls.SDET/src/Automation.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smartcontrolsin-my.sharepoint.com/personal/lohith_patil_smartcontrols_in/Documents/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{C8161079-A5D2-4217-AEC9-BB3DD410F45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F44ED76-58EF-4B3F-ADEB-4E703AE0838E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F2D70720-E269-402D-9348-F901CD303898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35895" yWindow="4260" windowWidth="28800" windowHeight="11235" xr2:uid="{6452F18F-7895-4B2D-8A43-7E46840F2AF0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{6452F18F-7895-4B2D-8A43-7E46840F2AF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,12 +32,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>DeprtmentGroupName</t>
   </si>
   <si>
     <t>Automation</t>
+  </si>
+  <si>
+    <t>Departments</t>
+  </si>
+  <si>
+    <t>AutomatonTest</t>
   </si>
 </sst>
 </file>
@@ -77,8 +79,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5162B0-3621-417E-80E6-F58D97FFD320}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,14 +429,20 @@
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>